<commit_message>
add status in rst_order table
</commit_message>
<xml_diff>
--- a/02 Documents/03 接口协议设计/Mobile接口.xlsx
+++ b/02 Documents/03 接口协议设计/Mobile接口.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="1" r:id="rId1"/>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1340,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1927,7 +1927,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>